<commit_message>
crop production and el nano updated
</commit_message>
<xml_diff>
--- a/elnino/elnano_data.xlsx
+++ b/elnino/elnano_data.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DC7826C-9580-437C-83FD-6E8AB173B31A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -63,7 +64,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -450,16 +451,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M76"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P17" sqref="P17"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="O76" sqref="O76"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -500,7 +501,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A2" s="1">
         <v>1950</v>
       </c>
@@ -541,7 +542,7 @@
         <v>-0.8</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A3" s="1">
         <v>1951</v>
       </c>
@@ -582,7 +583,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A4" s="1">
         <v>1952</v>
       </c>
@@ -623,7 +624,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A5" s="1">
         <v>1953</v>
       </c>
@@ -664,7 +665,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A6" s="1">
         <v>1954</v>
       </c>
@@ -705,7 +706,7 @@
         <v>-0.7</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A7" s="1">
         <v>1955</v>
       </c>
@@ -746,7 +747,7 @@
         <v>-1.5</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A8" s="1">
         <v>1956</v>
       </c>
@@ -787,7 +788,7 @@
         <v>-0.4</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A9" s="1">
         <v>1957</v>
       </c>
@@ -828,7 +829,7 @@
         <v>1.7</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A10" s="1">
         <v>1958</v>
       </c>
@@ -869,7 +870,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A11" s="1">
         <v>1959</v>
       </c>
@@ -910,7 +911,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A12" s="1">
         <v>1960</v>
       </c>
@@ -951,7 +952,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A13" s="1">
         <v>1961</v>
       </c>
@@ -992,7 +993,7 @@
         <v>-0.2</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A14" s="1">
         <v>1962</v>
       </c>
@@ -1033,7 +1034,7 @@
         <v>-0.4</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A15" s="1">
         <v>1963</v>
       </c>
@@ -1074,7 +1075,7 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A16" s="1">
         <v>1964</v>
       </c>
@@ -1115,7 +1116,7 @@
         <v>-0.8</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A17" s="1">
         <v>1965</v>
       </c>
@@ -1156,7 +1157,7 @@
         <v>1.7</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A18" s="1">
         <v>1966</v>
       </c>
@@ -1197,7 +1198,7 @@
         <v>-0.3</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A19" s="1">
         <v>1967</v>
       </c>
@@ -1238,7 +1239,7 @@
         <v>-0.4</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A20" s="1">
         <v>1968</v>
       </c>
@@ -1279,7 +1280,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A21" s="1">
         <v>1969</v>
       </c>
@@ -1320,7 +1321,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A22" s="1">
         <v>1970</v>
       </c>
@@ -1361,7 +1362,7 @@
         <v>-1.1000000000000001</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A23" s="1">
         <v>1971</v>
       </c>
@@ -1402,7 +1403,7 @@
         <v>-0.9</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A24" s="1">
         <v>1972</v>
       </c>
@@ -1443,7 +1444,7 @@
         <v>2.1</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A25" s="1">
         <v>1973</v>
       </c>
@@ -1484,7 +1485,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A26" s="1">
         <v>1974</v>
       </c>
@@ -1525,7 +1526,7 @@
         <v>-0.6</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A27" s="1">
         <v>1975</v>
       </c>
@@ -1566,7 +1567,7 @@
         <v>-1.7</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A28" s="1">
         <v>1976</v>
       </c>
@@ -1607,7 +1608,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A29" s="1">
         <v>1977</v>
       </c>
@@ -1648,7 +1649,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A30" s="1">
         <v>1978</v>
       </c>
@@ -1689,7 +1690,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A31" s="1">
         <v>1979</v>
       </c>
@@ -1730,7 +1731,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A32" s="1">
         <v>1980</v>
       </c>
@@ -1771,7 +1772,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A33" s="1">
         <v>1981</v>
       </c>
@@ -1812,7 +1813,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A34" s="1">
         <v>1982</v>
       </c>
@@ -1853,7 +1854,7 @@
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A35" s="1">
         <v>1983</v>
       </c>
@@ -1894,7 +1895,7 @@
         <v>-0.9</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A36" s="1">
         <v>1984</v>
       </c>
@@ -1935,7 +1936,7 @@
         <v>-1.1000000000000001</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A37" s="1">
         <v>1985</v>
       </c>
@@ -1976,7 +1977,7 @@
         <v>-0.4</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A38" s="1">
         <v>1986</v>
       </c>
@@ -2017,7 +2018,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A39" s="1">
         <v>1987</v>
       </c>
@@ -2058,7 +2059,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A40" s="1">
         <v>1988</v>
       </c>
@@ -2099,7 +2100,7 @@
         <v>-1.8</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A41" s="1">
         <v>1989</v>
       </c>
@@ -2140,7 +2141,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A42" s="1">
         <v>1990</v>
       </c>
@@ -2181,7 +2182,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A43" s="1">
         <v>1991</v>
       </c>
@@ -2222,7 +2223,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A44" s="1">
         <v>1992</v>
       </c>
@@ -2263,7 +2264,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A45" s="1">
         <v>1993</v>
       </c>
@@ -2304,7 +2305,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A46" s="1">
         <v>1994</v>
       </c>
@@ -2345,7 +2346,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A47" s="1">
         <v>1995</v>
       </c>
@@ -2386,7 +2387,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A48" s="1">
         <v>1996</v>
       </c>
@@ -2427,7 +2428,7 @@
         <v>-0.5</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A49" s="1">
         <v>1997</v>
       </c>
@@ -2468,7 +2469,7 @@
         <v>2.4</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A50" s="1">
         <v>1998</v>
       </c>
@@ -2509,7 +2510,7 @@
         <v>-1.6</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A51" s="1">
         <v>1999</v>
       </c>
@@ -2550,7 +2551,7 @@
         <v>-1.7</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A52" s="1">
         <v>2000</v>
       </c>
@@ -2591,7 +2592,7 @@
         <v>-0.7</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A53" s="1">
         <v>2001</v>
       </c>
@@ -2632,7 +2633,7 @@
         <v>-0.3</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A54" s="1">
         <v>2002</v>
       </c>
@@ -2673,7 +2674,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A55" s="1">
         <v>2003</v>
       </c>
@@ -2714,7 +2715,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A56" s="1">
         <v>2004</v>
       </c>
@@ -2755,7 +2756,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A57" s="1">
         <v>2005</v>
       </c>
@@ -2796,7 +2797,7 @@
         <v>-0.8</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A58" s="1">
         <v>2006</v>
       </c>
@@ -2837,7 +2838,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A59" s="1">
         <v>2007</v>
       </c>
@@ -2878,7 +2879,7 @@
         <v>-1.6</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A60" s="1">
         <v>2008</v>
       </c>
@@ -2919,7 +2920,7 @@
         <v>-0.7</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A61" s="1">
         <v>2009</v>
       </c>
@@ -2960,7 +2961,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A62" s="1">
         <v>2010</v>
       </c>
@@ -3001,7 +3002,7 @@
         <v>-1.6</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A63" s="1">
         <v>2011</v>
       </c>
@@ -3042,7 +3043,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A64" s="1">
         <v>2012</v>
       </c>
@@ -3083,7 +3084,7 @@
         <v>-0.2</v>
       </c>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A65" s="1">
         <v>2013</v>
       </c>
@@ -3124,7 +3125,7 @@
         <v>-0.3</v>
       </c>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A66" s="1">
         <v>2014</v>
       </c>
@@ -3165,7 +3166,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A67" s="1">
         <v>2015</v>
       </c>
@@ -3206,7 +3207,7 @@
         <v>2.6</v>
       </c>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A68" s="1">
         <v>2016</v>
       </c>
@@ -3247,7 +3248,7 @@
         <v>-0.6</v>
       </c>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A69" s="1">
         <v>2017</v>
       </c>
@@ -3288,7 +3289,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A70" s="1">
         <v>2018</v>
       </c>
@@ -3329,7 +3330,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A71" s="1">
         <v>2019</v>
       </c>
@@ -3370,7 +3371,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A72" s="1">
         <v>2020</v>
       </c>
@@ -3411,7 +3412,7 @@
         <v>-1.2</v>
       </c>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A73" s="1">
         <v>2021</v>
       </c>
@@ -3452,7 +3453,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A74" s="1">
         <v>2022</v>
       </c>
@@ -3493,7 +3494,7 @@
         <v>-0.8</v>
       </c>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A75" s="1">
         <v>2023</v>
       </c>
@@ -3534,7 +3535,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A76" s="1">
         <v>2024</v>
       </c>
@@ -3547,15 +3548,33 @@
       <c r="D76" s="4">
         <v>1.1000000000000001</v>
       </c>
-      <c r="E76" s="5"/>
-      <c r="F76" s="5"/>
-      <c r="G76" s="5"/>
-      <c r="H76" s="5"/>
-      <c r="I76" s="5"/>
-      <c r="J76" s="5"/>
-      <c r="K76" s="5"/>
-      <c r="L76" s="5"/>
-      <c r="M76" s="6"/>
+      <c r="E76" s="5">
+        <v>0.7</v>
+      </c>
+      <c r="F76" s="5">
+        <v>0.4</v>
+      </c>
+      <c r="G76" s="5">
+        <v>0</v>
+      </c>
+      <c r="H76" s="5">
+        <v>0</v>
+      </c>
+      <c r="I76" s="5">
+        <v>0</v>
+      </c>
+      <c r="J76" s="5">
+        <v>0</v>
+      </c>
+      <c r="K76" s="5">
+        <v>0</v>
+      </c>
+      <c r="L76" s="5">
+        <v>0</v>
+      </c>
+      <c r="M76" s="6">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>